<commit_message>
Updated template to contain new formulas which show the monthly and yearly validation values.
</commit_message>
<xml_diff>
--- a/src/SFA.DAS.EmployerIncentives.Database/Scripts/Metrics Template.xlsx
+++ b/src/SFA.DAS.EmployerIncentives.Database/Scripts/Metrics Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\das-employer-incentives\src\SFA.DAS.EmployerIncentives.Database\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19294C0E-8EE5-4E1E-84CB-56498659CD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901E936F-E637-4EED-BA1E-89CE2A7E2C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8544" yWindow="-4362" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{D09B5AF9-3A6F-42DB-93C1-FBFD14450138}"/>
+    <workbookView xWindow="8544" yWindow="-4362" windowWidth="23232" windowHeight="12552" xr2:uid="{D09B5AF9-3A6F-42DB-93C1-FBFD14450138}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="8" r:id="rId1"/>
@@ -228,7 +228,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="D29" authorId="0" shapeId="0" xr:uid="{394124AF-C135-4606-BE93-DCB5B7D6E042}">
+    <comment ref="A32" authorId="0" shapeId="0" xr:uid="{0D5D5CB3-E2C4-4A24-A0C1-79B4539F9269}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>David Steele:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Paid vs Validation fails</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D33" authorId="0" shapeId="0" xr:uid="{394124AF-C135-4606-BE93-DCB5B7D6E042}">
       <text>
         <r>
           <rPr>
@@ -253,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A32" authorId="0" shapeId="0" xr:uid="{7347AAF6-F364-4813-BDA8-F41A2444DE03}">
+    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{7347AAF6-F364-4813-BDA8-F41A2444DE03}">
       <text>
         <r>
           <rPr>
@@ -424,7 +448,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>CountOfPayments</t>
   </si>
@@ -495,9 +519,6 @@
     <t>Total validated</t>
   </si>
   <si>
-    <t>Accounted for Earnings</t>
-  </si>
-  <si>
     <t>Difference</t>
   </si>
   <si>
@@ -525,9 +546,6 @@
     <t>Percentage of validation records paid</t>
   </si>
   <si>
-    <t>Send</t>
-  </si>
-  <si>
     <t>Unsent</t>
   </si>
   <si>
@@ -544,6 +562,15 @@
   </si>
   <si>
     <t>Num Legal Entity IDs</t>
+  </si>
+  <si>
+    <t>Earnings Sub-total</t>
+  </si>
+  <si>
+    <t>Accounted for earnings</t>
+  </si>
+  <si>
+    <t>Sent</t>
   </si>
 </sst>
 </file>
@@ -554,7 +581,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -619,6 +646,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -648,14 +688,13 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -678,6 +717,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -994,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CF0EC6D-C2B4-4297-9222-9B55C26E2BD6}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,7 +1059,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1">
         <v>10</v>
@@ -1026,7 +1068,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>2021</v>
@@ -1048,7 +1090,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1059,7 +1101,7 @@
       <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="14"/>
       <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1080,7 +1122,7 @@
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="8"/>
       <c r="F6" s="2"/>
       <c r="G6">
         <v>3</v>
@@ -1097,7 +1139,7 @@
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="8"/>
       <c r="F7" s="2"/>
       <c r="G7">
         <v>4</v>
@@ -1114,7 +1156,7 @@
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="8"/>
       <c r="F8" s="2"/>
       <c r="G8">
         <v>5</v>
@@ -1131,7 +1173,7 @@
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="8"/>
       <c r="F9" s="2"/>
       <c r="G9">
         <v>6</v>
@@ -1148,7 +1190,7 @@
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="8"/>
       <c r="F10" s="2"/>
       <c r="G10">
         <v>7</v>
@@ -1165,7 +1207,7 @@
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="D11" s="9"/>
+      <c r="D11" s="8"/>
       <c r="F11" s="2"/>
       <c r="G11">
         <v>8</v>
@@ -1182,7 +1224,7 @@
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="D12" s="9"/>
+      <c r="D12" s="8"/>
       <c r="G12">
         <v>9</v>
       </c>
@@ -1199,7 +1241,7 @@
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="D13" s="9"/>
+      <c r="D13" s="8"/>
       <c r="G13">
         <v>10</v>
       </c>
@@ -1215,7 +1257,7 @@
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="D14" s="9"/>
+      <c r="D14" s="8"/>
       <c r="G14">
         <v>11</v>
       </c>
@@ -1231,7 +1273,7 @@
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="D15" s="9"/>
+      <c r="D15" s="8"/>
       <c r="G15">
         <v>12</v>
       </c>
@@ -1247,7 +1289,7 @@
       <c r="B16">
         <v>3</v>
       </c>
-      <c r="D16" s="9"/>
+      <c r="D16" s="8"/>
       <c r="G16">
         <v>1</v>
       </c>
@@ -1263,8 +1305,8 @@
       <c r="B17">
         <v>4</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="F17" s="10"/>
+      <c r="D17" s="8"/>
+      <c r="F17" s="9"/>
       <c r="G17">
         <v>2</v>
       </c>
@@ -1275,17 +1317,17 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="1">
         <f>SUM(C6:C17)</f>
         <v>0</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="19">
         <f>SUM(D6:D17)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="10"/>
+      <c r="F18" s="9"/>
       <c r="G18">
         <v>3</v>
       </c>
@@ -1296,7 +1338,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="4" t="e">
         <f>SUMIFS(D6:D17,B6:B17,"="&amp;B1,A6:A17,B2)/D22</f>
@@ -1312,7 +1354,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
-      <c r="F20" s="9"/>
+      <c r="F20" s="8"/>
       <c r="G20">
         <v>5</v>
       </c>
@@ -1334,16 +1376,16 @@
         <v>R10</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="18"/>
+        <v>25</v>
+      </c>
+      <c r="F21" s="17"/>
       <c r="G21">
         <v>6</v>
       </c>
       <c r="H21">
         <v>2122</v>
       </c>
-      <c r="I21" s="9"/>
+      <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -1353,19 +1395,19 @@
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="21">
+      <c r="D22" s="9"/>
+      <c r="E22" s="20">
         <f>'YTD Validation'!L37</f>
         <v>0</v>
       </c>
-      <c r="F22" s="17"/>
+      <c r="F22" s="16"/>
       <c r="G22">
         <v>7</v>
       </c>
       <c r="H22">
         <v>2122</v>
       </c>
-      <c r="I22" s="9"/>
+      <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -1374,42 +1416,42 @@
       <c r="C23">
         <v>0</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="21">
+      <c r="D23" s="9"/>
+      <c r="E23" s="20">
         <f>SUM('YTD Validation'!L38:L78)</f>
         <v>0</v>
       </c>
-      <c r="F23" s="17"/>
+      <c r="F23" s="16"/>
       <c r="G23">
         <v>8</v>
       </c>
       <c r="H23">
         <v>2122</v>
       </c>
-      <c r="I23" s="9"/>
+      <c r="I23" s="8"/>
       <c r="M23" s="2"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="19">
         <f>SUM(D22:D23)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="28">
         <f>SUM(E22:E23)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="16"/>
+      <c r="F24" s="15"/>
       <c r="G24">
         <v>9</v>
       </c>
       <c r="H24">
         <v>2122</v>
       </c>
-      <c r="I24" s="9"/>
+      <c r="I24" s="8"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
@@ -1420,30 +1462,30 @@
       <c r="H25">
         <v>2122</v>
       </c>
-      <c r="I25" s="9"/>
+      <c r="I25" s="8"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="10"/>
+      <c r="F26" s="9"/>
       <c r="G26">
         <v>11</v>
       </c>
       <c r="H26">
         <v>2122</v>
       </c>
-      <c r="I26" s="9"/>
+      <c r="I26" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="str">
         <f>"R" &amp; B1 &amp; " YTD Earnings"</f>
         <v>R10 YTD Earnings</v>
       </c>
-      <c r="D27" s="2">
+      <c r="E27" s="2">
         <f>SUMIFS(I6:I29,G6:G29,"&lt;="&amp;B1,H6:H29,B2)</f>
         <v>0</v>
       </c>
@@ -1453,14 +1495,14 @@
       <c r="H27">
         <v>2122</v>
       </c>
-      <c r="I27" s="9"/>
+      <c r="I27" s="8"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="2">
-        <f>D27-E24</f>
+        <v>26</v>
+      </c>
+      <c r="E28" s="8">
+        <f>D38</f>
         <v>0</v>
       </c>
       <c r="G28">
@@ -1469,16 +1511,18 @@
       <c r="H28">
         <v>2223</v>
       </c>
-      <c r="I28" s="9"/>
+      <c r="I28" s="8"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6" t="e">
-        <f>D28/D27</f>
-        <v>#DIV/0!</v>
+      <c r="A29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="19">
+        <f>E27+E28</f>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>2</v>
@@ -1486,24 +1530,72 @@
       <c r="H29">
         <v>2223</v>
       </c>
-      <c r="I29" s="9"/>
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="26"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="10">
-        <v>-532750</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="2"/>
+      <c r="A32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="19">
+        <f>D18+D23</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="19">
+        <f>E24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27" t="e">
+        <f>D32/E32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E33" s="19">
+        <f>E32-D32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="19">
+        <f>SUM(D36:D37)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1516,7 +1608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E57346C4-B56D-4D76-8149-BD4AE249F3F4}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1532,82 +1624,82 @@
     <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="19" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="18" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" style="8" customWidth="1"/>
     <col min="14" max="14" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H1" s="3"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="26"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="25"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="22"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="21"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H5" s="3"/>
@@ -1658,17 +1750,17 @@
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="25"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="24"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H22" s="3"/>
@@ -1705,7 +1797,7 @@
     </row>
     <row r="35" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1734,52 +1826,52 @@
         <v>11</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K36" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="L36" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K36" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L36" s="8" t="s">
         <v>7</v>
       </c>
       <c r="O36" s="2"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="26"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="25"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="23"/>
-    </row>
-    <row r="46" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="23"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="22"/>
+    </row>
+    <row r="46" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="22"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:O2" xr:uid="{E57346C4-B56D-4D76-8149-BD4AE249F3F4}"/>
@@ -1802,15 +1894,53 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2">342KH2PRRWRA-1278990367-2</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2">
-      <Url>https://educationgovuk.sharepoint.com/sites/lveesfa00044/_layouts/15/DocIdRedir.aspx?ID=342KH2PRRWRA-1278990367-2</Url>
-      <Description>342KH2PRRWRA-1278990367-2</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1976,53 +2106,15 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2">342KH2PRRWRA-1278990367-2</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2">
+      <Url>https://educationgovuk.sharepoint.com/sites/lveesfa00044/_layouts/15/DocIdRedir.aspx?ID=342KH2PRRWRA-1278990367-2</Url>
+      <Description>342KH2PRRWRA-1278990367-2</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2034,11 +2126,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{338C00EC-A99B-4DDF-9B0D-B919A174C184}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3B6D462-9A8A-45BE-A3C6-59EEC4C4A7AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2063,9 +2153,11 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3B6D462-9A8A-45BE-A3C6-59EEC4C4A7AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{338C00EC-A99B-4DDF-9B0D-B919A174C184}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
EI-1709 removed formulae from cells E22, E23
</commit_message>
<xml_diff>
--- a/src/SFA.DAS.EmployerIncentives.Database/Scripts/Metrics Template.xlsx
+++ b/src/SFA.DAS.EmployerIncentives.Database/Scripts/Metrics Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\das-employer-incentives\src\SFA.DAS.EmployerIncentives.Database\Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESFA\das-employer-incentives\src\SFA.DAS.EmployerIncentives.Database\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901E936F-E637-4EED-BA1E-89CE2A7E2C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B72F9A-7FDF-4BCE-ACC2-78247F025D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8544" yWindow="-4362" windowWidth="23232" windowHeight="12552" xr2:uid="{D09B5AF9-3A6F-42DB-93C1-FBFD14450138}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D09B5AF9-3A6F-42DB-93C1-FBFD14450138}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="8" r:id="rId1"/>
@@ -19,10 +19,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'YTD Validation'!$A$2:$M$2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1039,25 +1049,25 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" customWidth="1"/>
-    <col min="6" max="7" width="17.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35.44140625" customWidth="1"/>
+    <col min="6" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1066,7 +1076,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1074,11 +1084,11 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1088,7 +1098,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -1115,7 +1125,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -1132,7 +1142,7 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2021</v>
       </c>
@@ -1149,7 +1159,7 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2021</v>
       </c>
@@ -1166,7 +1176,7 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2021</v>
       </c>
@@ -1183,7 +1193,7 @@
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2021</v>
       </c>
@@ -1200,7 +1210,7 @@
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2021</v>
       </c>
@@ -1217,7 +1227,7 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2021</v>
       </c>
@@ -1234,7 +1244,7 @@
       <c r="I12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -1250,7 +1260,7 @@
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2021</v>
       </c>
@@ -1266,7 +1276,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -1282,7 +1292,7 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2021</v>
       </c>
@@ -1298,7 +1308,7 @@
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2021</v>
       </c>
@@ -1315,7 +1325,7 @@
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1336,7 +1346,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1352,7 +1362,7 @@
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D20" s="4"/>
       <c r="F20" s="8"/>
       <c r="G20">
@@ -1363,7 +1373,7 @@
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1387,7 +1397,7 @@
       </c>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>17</v>
       </c>
@@ -1396,10 +1406,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="20">
-        <f>'YTD Validation'!L37</f>
-        <v>0</v>
-      </c>
+      <c r="E22" s="20"/>
       <c r="F22" s="16"/>
       <c r="G22">
         <v>7</v>
@@ -1409,7 +1416,7 @@
       </c>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>20</v>
       </c>
@@ -1417,10 +1424,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="9"/>
-      <c r="E23" s="20">
-        <f>SUM('YTD Validation'!L38:L78)</f>
-        <v>0</v>
-      </c>
+      <c r="E23" s="20"/>
       <c r="F23" s="16"/>
       <c r="G23">
         <v>8</v>
@@ -1431,7 +1435,7 @@
       <c r="I23" s="8"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>22</v>
@@ -1453,7 +1457,7 @@
       </c>
       <c r="I24" s="8"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="D25" s="2"/>
       <c r="G25">
@@ -1464,7 +1468,7 @@
       </c>
       <c r="I25" s="8"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
@@ -1480,7 +1484,7 @@
       </c>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="str">
         <f>"R" &amp; B1 &amp; " YTD Earnings"</f>
         <v>R10 YTD Earnings</v>
@@ -1497,7 +1501,7 @@
       </c>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
@@ -1513,7 +1517,7 @@
       </c>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
@@ -1532,15 +1536,15 @@
       </c>
       <c r="I29" s="8"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="D30" s="2"/>
       <c r="E30" s="26"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
@@ -1555,7 +1559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>23</v>
       </c>
@@ -1570,7 +1574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -1580,14 +1584,14 @@
       <c r="D36" s="9"/>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
         <v>32</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C38" s="1" t="s">
         <v>30</v>
       </c>
@@ -1612,31 +1616,31 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="18" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" style="8" customWidth="1"/>
-    <col min="14" max="14" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="18" customWidth="1"/>
+    <col min="12" max="12" width="22.109375" style="8" customWidth="1"/>
+    <col min="14" max="14" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H1" s="3"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1674,7 +1678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -1688,7 +1692,7 @@
       <c r="K3" s="23"/>
       <c r="L3" s="25"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1701,55 +1705,55 @@
       <c r="J4" s="7"/>
       <c r="K4" s="21"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1762,45 +1766,45 @@
       <c r="J21" s="13"/>
       <c r="K21" s="24"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H32" s="3"/>
     </row>
-    <row r="35" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -1839,7 +1843,7 @@
       </c>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -1853,7 +1857,7 @@
       <c r="K37" s="23"/>
       <c r="L37" s="25"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1867,7 +1871,7 @@
       <c r="K39" s="21"/>
       <c r="L39" s="22"/>
     </row>
-    <row r="46" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
       <c r="K46" s="21"/>
@@ -1885,65 +1889,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2">342KH2PRRWRA-1278990367-2</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2">
+      <Url>https://educationgovuk.sharepoint.com/sites/lveesfa00044/_layouts/15/DocIdRedir.aspx?ID=342KH2PRRWRA-1278990367-2</Url>
+      <Description>342KH2PRRWRA-1278990367-2</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100943E1C22BFE883409EEBD231A3511F28" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1c945f1aad39a0eeba24ecd9a3efacb6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2" xmlns:ns3="4ab9d8d1-3ef6-4dd7-8d9b-7b80fa9385d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="17569109299e627b73b1409a5cfb546a" ns2:_="" ns3:_="">
     <xsd:import namespace="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2"/>
@@ -2105,35 +2062,76 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2">342KH2PRRWRA-1278990367-2</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2">
-      <Url>https://educationgovuk.sharepoint.com/sites/lveesfa00044/_layouts/15/DocIdRedir.aspx?ID=342KH2PRRWRA-1278990367-2</Url>
-      <Description>342KH2PRRWRA-1278990367-2</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E86AC837-6146-4448-8D80-355E71DFBC39}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{338C00EC-A99B-4DDF-9B0D-B919A174C184}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3B6D462-9A8A-45BE-A3C6-59EEC4C4A7AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07A08636-6383-4039-A929-8E85D0719125}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2152,12 +2150,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3B6D462-9A8A-45BE-A3C6-59EEC4C4A7AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{338C00EC-A99B-4DDF-9B0D-B919A174C184}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E86AC837-6146-4448-8D80-355E71DFBC39}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
EI-1709 update accounted for earnings total to only include current AY
</commit_message>
<xml_diff>
--- a/src/SFA.DAS.EmployerIncentives.Database/Scripts/Metrics Template.xlsx
+++ b/src/SFA.DAS.EmployerIncentives.Database/Scripts/Metrics Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESFA\das-employer-incentives\src\SFA.DAS.EmployerIncentives.Database\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B72F9A-7FDF-4BCE-ACC2-78247F025D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D59C1CC-EDE5-48E8-BC3B-71475CAD319D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D09B5AF9-3A6F-42DB-93C1-FBFD14450138}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D09B5AF9-3A6F-42DB-93C1-FBFD14450138}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="8" r:id="rId1"/>
@@ -42,6 +42,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>David Steele</author>
+    <author>tc={ECAEACAD-CA4F-4F96-8EDA-0C31F5A4A8F3}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{DDA48418-12E8-4A8B-A314-CE0BD5CA91AF}">
@@ -260,6 +261,14 @@
           <t xml:space="preserve">
 Paid vs Validation fails</t>
         </r>
+      </text>
+    </comment>
+    <comment ref="D32" authorId="1" shapeId="0" xr:uid="{ECAEACAD-CA4F-4F96-8EDA-0C31F5A4A8F3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This value should be the sum of payment amounts for the current Academic Year</t>
       </text>
     </comment>
     <comment ref="D33" authorId="0" shapeId="0" xr:uid="{394124AF-C135-4606-BE93-DCB5B7D6E042}">
@@ -747,6 +756,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Dave Read" id="{433A4255-8BF5-4AE5-B78B-B7002F0085E4}" userId="1c4ee2a5303dc2ae" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1044,12 +1059,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D32" dT="2022-03-30T14:14:41.66" personId="{433A4255-8BF5-4AE5-B78B-B7002F0085E4}" id="{ECAEACAD-CA4F-4F96-8EDA-0C31F5A4A8F3}">
+    <text>This value should be the sum of payment amounts for the current Academic Year</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CF0EC6D-C2B4-4297-9222-9B55C26E2BD6}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1551,7 +1574,7 @@
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="19">
-        <f>D18+D23</f>
+        <f>SUM(D14:D18)+D23</f>
         <v>0</v>
       </c>
       <c r="E32" s="19">
@@ -1901,6 +1924,65 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100943E1C22BFE883409EEBD231A3511F28" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1c945f1aad39a0eeba24ecd9a3efacb6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2" xmlns:ns3="4ab9d8d1-3ef6-4dd7-8d9b-7b80fa9385d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="17569109299e627b73b1409a5cfb546a" ns2:_="" ns3:_="">
     <xsd:import namespace="ba2294b9-6d6a-4c9b-a125-9e4b98f52ed2"/>
@@ -2062,65 +2144,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{338C00EC-A99B-4DDF-9B0D-B919A174C184}">
   <ds:schemaRefs>
@@ -2132,6 +2155,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E86AC837-6146-4448-8D80-355E71DFBC39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3B6D462-9A8A-45BE-A3C6-59EEC4C4A7AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07A08636-6383-4039-A929-8E85D0719125}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2148,20 +2187,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3B6D462-9A8A-45BE-A3C6-59EEC4C4A7AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E86AC837-6146-4448-8D80-355E71DFBC39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>